<commit_message>
almost done refactoring v4 link MCU schematic
</commit_message>
<xml_diff>
--- a/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_LINK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C763CA-1F5A-4F5A-9FBA-1264D6F63DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE51C2-31E0-4170-AD0C-1331494D8767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>PIN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="90">
   <si>
     <t>SPI</t>
   </si>
@@ -48,6 +45,267 @@
   </si>
   <si>
     <t>GPIO</t>
+  </si>
+  <si>
+    <t>PIN NAME</t>
+  </si>
+  <si>
+    <t>PIN NUM</t>
+  </si>
+  <si>
+    <t>PC13</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>PC0</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>LPUART1_RX</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>LPUART1_TX</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>MAX V</t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>USART2_TX</t>
+  </si>
+  <si>
+    <t>PA3</t>
+  </si>
+  <si>
+    <t>USART2_RX</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>SPI1/3_NSS</t>
+  </si>
+  <si>
+    <t>PA5</t>
+  </si>
+  <si>
+    <t>PA7</t>
+  </si>
+  <si>
+    <t>PA6</t>
+  </si>
+  <si>
+    <t>SPI1_SCLK</t>
+  </si>
+  <si>
+    <t>SPI1_MISO</t>
+  </si>
+  <si>
+    <t>SPI1_MOSI</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>USART1_TX</t>
+  </si>
+  <si>
+    <t>PC5</t>
+  </si>
+  <si>
+    <t>USART1_RX</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>PB2</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>USART3_TX</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>USART3_RX</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>SPI2_NSS</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>FDCAN2_RX</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>SPI2_SCLK</t>
+  </si>
+  <si>
+    <t>FDCAN2_TX</t>
+  </si>
+  <si>
+    <t>PB14</t>
+  </si>
+  <si>
+    <t>SPI2_MISO</t>
+  </si>
+  <si>
+    <t>PB15</t>
+  </si>
+  <si>
+    <t>SPI2_MOSI</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
+    <t>PC9</t>
+  </si>
+  <si>
+    <t>PA8</t>
+  </si>
+  <si>
+    <t>FDCAN3_RX</t>
+  </si>
+  <si>
+    <t>PA9</t>
+  </si>
+  <si>
+    <t>PA10</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>FDCAN1_RX</t>
+  </si>
+  <si>
+    <t>PA12</t>
+  </si>
+  <si>
+    <t>FDCAN1_TX</t>
+  </si>
+  <si>
+    <t>PA13</t>
+  </si>
+  <si>
+    <t>SWDIO</t>
+  </si>
+  <si>
+    <t>PA14</t>
+  </si>
+  <si>
+    <t>SWCLK</t>
+  </si>
+  <si>
+    <t>PA15</t>
+  </si>
+  <si>
+    <t>FDCAN3_TX</t>
+  </si>
+  <si>
+    <t>PC10</t>
+  </si>
+  <si>
+    <t>SPI3_SCLK</t>
+  </si>
+  <si>
+    <t>USART3/4_TX</t>
+  </si>
+  <si>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>SPI3_MISO</t>
+  </si>
+  <si>
+    <t>USART3/4_RX</t>
+  </si>
+  <si>
+    <t>PC12</t>
+  </si>
+  <si>
+    <t>SPI3_MOSI</t>
+  </si>
+  <si>
+    <t>UART5_TX</t>
+  </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>UART5_RX</t>
+  </si>
+  <si>
+    <t>PB3</t>
+  </si>
+  <si>
+    <t>SWO</t>
+  </si>
+  <si>
+    <t>PB4</t>
+  </si>
+  <si>
+    <t>SPI1/3_MISO</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>SPI1/3_MOSI</t>
+  </si>
+  <si>
+    <t>PB6</t>
+  </si>
+  <si>
+    <t>PB7</t>
+  </si>
+  <si>
+    <t>PB8</t>
+  </si>
+  <si>
+    <t>PB9</t>
   </si>
 </sst>
 </file>
@@ -83,8 +341,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,29 +680,949 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>56</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>57</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G43" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>62</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" t="s">
+        <v>62</v>
+      </c>
+      <c r="G48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C42:G42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
halfway thru working on link layout
</commit_message>
<xml_diff>
--- a/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_LINK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE51C2-31E0-4170-AD0C-1331494D8767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF33433B-192D-4489-BCC1-7BB7E3341F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
+    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="99">
   <si>
     <t>SPI</t>
   </si>
@@ -306,6 +306,33 @@
   </si>
   <si>
     <t>PB9</t>
+  </si>
+  <si>
+    <t>HYDRA_V3_LINK</t>
+  </si>
+  <si>
+    <t>ETH_NSS</t>
+  </si>
+  <si>
+    <t>ETH_SCLK</t>
+  </si>
+  <si>
+    <t>ETH_MISO</t>
+  </si>
+  <si>
+    <t>ETH_MOSI</t>
+  </si>
+  <si>
+    <t>ETH_NRST</t>
+  </si>
+  <si>
+    <t>ETH_NINT</t>
+  </si>
+  <si>
+    <t>RFD TX</t>
+  </si>
+  <si>
+    <t>RFD RX</t>
   </si>
 </sst>
 </file>
@@ -321,12 +348,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -341,11 +374,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,25 +715,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -723,8 +760,11 @@
       <c r="H1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -738,7 +778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -758,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -778,7 +818,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -795,7 +835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11</v>
       </c>
@@ -812,7 +852,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12</v>
       </c>
@@ -829,7 +869,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>13</v>
       </c>
@@ -846,7 +886,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
@@ -866,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -886,7 +926,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>
@@ -905,8 +945,11 @@
       <c r="H11">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J11" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>19</v>
       </c>
@@ -925,8 +968,11 @@
       <c r="H12">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J12" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20</v>
       </c>
@@ -945,8 +991,11 @@
       <c r="H13">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J13" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -965,8 +1014,11 @@
       <c r="H14">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>22</v>
       </c>
@@ -985,8 +1037,11 @@
       <c r="H15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>23</v>
       </c>
@@ -1005,8 +1060,11 @@
       <c r="H16">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>24</v>
       </c>
@@ -1023,7 +1081,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>25</v>
       </c>
@@ -1040,7 +1098,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>26</v>
       </c>
@@ -1057,7 +1115,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30</v>
       </c>
@@ -1074,7 +1132,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>33</v>
       </c>
@@ -1094,7 +1152,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>34</v>
       </c>
@@ -1117,7 +1175,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>35</v>
       </c>
@@ -1140,7 +1198,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>36</v>
       </c>
@@ -1160,7 +1218,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>37</v>
       </c>
@@ -1180,7 +1238,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>38</v>
       </c>
@@ -1197,7 +1255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>39</v>
       </c>
@@ -1214,7 +1272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>40</v>
       </c>
@@ -1231,7 +1289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>41</v>
       </c>
@@ -1248,7 +1306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>42</v>
       </c>
@@ -1268,7 +1326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>43</v>
       </c>
@@ -1285,7 +1343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>44</v>
       </c>
@@ -1305,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>45</v>
       </c>
@@ -1325,7 +1383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>46</v>
       </c>
@@ -1342,7 +1400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>49</v>
       </c>
@@ -1359,8 +1417,11 @@
       <c r="H35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>50</v>
       </c>
@@ -1377,8 +1438,11 @@
       <c r="H36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>51</v>
       </c>
@@ -1401,7 +1465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>52</v>
       </c>
@@ -1421,7 +1485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>53</v>
       </c>
@@ -1441,7 +1505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>54</v>
       </c>
@@ -1460,8 +1524,11 @@
       <c r="H40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>55</v>
       </c>
@@ -1477,8 +1544,11 @@
       <c r="H41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>56</v>
       </c>
@@ -1495,8 +1565,11 @@
       <c r="H42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>57</v>
       </c>
@@ -1519,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>58</v>
       </c>
@@ -1539,7 +1612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>59</v>
       </c>
@@ -1559,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>60</v>
       </c>
@@ -1576,7 +1649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>61</v>
       </c>
@@ -1596,7 +1669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
almost done hydra v4 link layout, still missing red pwr led mosfet integration in schematics tho
</commit_message>
<xml_diff>
--- a/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_LINK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF33433B-192D-4489-BCC1-7BB7E3341F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB0DE51-B1CC-42EA-823D-0A76293AFCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="110">
   <si>
     <t>SPI</t>
   </si>
@@ -333,6 +333,39 @@
   </si>
   <si>
     <t>RFD RX</t>
+  </si>
+  <si>
+    <t>CAN0_RX</t>
+  </si>
+  <si>
+    <t>CAN0_TX</t>
+  </si>
+  <si>
+    <t>TCAN1146_nCS</t>
+  </si>
+  <si>
+    <t>CAN1_RX</t>
+  </si>
+  <si>
+    <t>CAN1_TX</t>
+  </si>
+  <si>
+    <t>SD_nCS</t>
+  </si>
+  <si>
+    <t>SD_SCLK</t>
+  </si>
+  <si>
+    <t>SD_MISO</t>
+  </si>
+  <si>
+    <t>SD_MOSI</t>
+  </si>
+  <si>
+    <t>SD_nCD</t>
+  </si>
+  <si>
+    <t>LORA_nCS</t>
   </si>
 </sst>
 </file>
@@ -348,7 +381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +391,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,13 +413,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +775,7 @@
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -771,11 +815,14 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H2">
         <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -862,7 +909,7 @@
       <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H7">
@@ -933,19 +980,19 @@
       <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H11">
         <v>3.6</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -956,7 +1003,7 @@
       <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F12" t="s">
@@ -968,7 +1015,7 @@
       <c r="H12">
         <v>3.6</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -979,7 +1026,7 @@
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F13" t="s">
@@ -991,7 +1038,7 @@
       <c r="H13">
         <v>3.6</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1002,7 +1049,7 @@
       <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F14" t="s">
@@ -1014,7 +1061,7 @@
       <c r="H14">
         <v>3.6</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1031,7 +1078,7 @@
       <c r="F15" t="s">
         <v>8</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H15">
@@ -1054,7 +1101,7 @@
       <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H16">
@@ -1064,7 +1111,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>24</v>
       </c>
@@ -1081,7 +1128,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>25</v>
       </c>
@@ -1098,7 +1145,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>26</v>
       </c>
@@ -1115,7 +1162,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30</v>
       </c>
@@ -1132,7 +1179,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>33</v>
       </c>
@@ -1145,21 +1192,24 @@
       <c r="F21" t="s">
         <v>8</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H21">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E22" t="s">
@@ -1174,15 +1224,18 @@
       <c r="H22">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E23" t="s">
@@ -1197,15 +1250,18 @@
       <c r="H23">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F24" t="s">
@@ -1217,15 +1273,18 @@
       <c r="H24">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F25" t="s">
@@ -1237,8 +1296,11 @@
       <c r="H25">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>38</v>
       </c>
@@ -1255,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>39</v>
       </c>
@@ -1272,7 +1334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>40</v>
       </c>
@@ -1289,7 +1351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>41</v>
       </c>
@@ -1306,7 +1368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>42</v>
       </c>
@@ -1326,7 +1388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>43</v>
       </c>
@@ -1343,7 +1405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>44</v>
       </c>
@@ -1407,13 +1469,13 @@
       <c r="B35" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
       <c r="H35">
         <v>5</v>
       </c>
@@ -1428,13 +1490,13 @@
       <c r="B36" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
       <c r="H36">
         <v>5</v>
       </c>
@@ -1449,7 +1511,7 @@
       <c r="B37" t="s">
         <v>67</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D37" t="s">
@@ -1472,7 +1534,7 @@
       <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="6" t="s">
         <v>70</v>
       </c>
       <c r="D38" t="s">
@@ -1492,7 +1554,7 @@
       <c r="B39" t="s">
         <v>72</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D39" t="s">
@@ -1515,7 +1577,7 @@
       <c r="C40" t="s">
         <v>76</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="4" t="s">
         <v>77</v>
       </c>
       <c r="G40" t="s">
@@ -1535,7 +1597,7 @@
       <c r="B41" t="s">
         <v>78</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G41" t="s">
@@ -1555,13 +1617,13 @@
       <c r="B42" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
       <c r="H42">
         <v>5</v>
       </c>
@@ -1585,11 +1647,14 @@
       <c r="E43" t="s">
         <v>68</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H43">
         <v>5</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1599,10 +1664,10 @@
       <c r="B44" t="s">
         <v>84</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="4" t="s">
         <v>43</v>
       </c>
       <c r="G44" t="s">
@@ -1610,6 +1675,9 @@
       </c>
       <c r="H44">
         <v>5</v>
+      </c>
+      <c r="J44" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1622,7 +1690,7 @@
       <c r="D45" t="s">
         <v>30</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G45" t="s">
@@ -1630,6 +1698,9 @@
       </c>
       <c r="H45">
         <v>5</v>
+      </c>
+      <c r="J45" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -1659,7 +1730,7 @@
       <c r="D47" t="s">
         <v>39</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G47" t="s">
@@ -1667,6 +1738,9 @@
       </c>
       <c r="H47">
         <v>5</v>
+      </c>
+      <c r="J47" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -1679,7 +1753,7 @@
       <c r="D48" t="s">
         <v>37</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G48" t="s">
@@ -1687,6 +1761,9 @@
       </c>
       <c r="H48">
         <v>5</v>
+      </c>
+      <c r="J48" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
link is hella populated, there are a few GPIOs left but trace width all around (excluding power traces) should be reduced to .15mm or less
</commit_message>
<xml_diff>
--- a/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_LINK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB0DE51-B1CC-42EA-823D-0A76293AFCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AD3A49-2D60-44C2-817A-37A83A6D2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="124">
   <si>
     <t>SPI</t>
   </si>
@@ -366,6 +366,48 @@
   </si>
   <si>
     <t>LORA_nCS</t>
+  </si>
+  <si>
+    <t>HYDRA_5V_V_SENSE</t>
+  </si>
+  <si>
+    <t>HYDRA_5V_I_SENSE</t>
+  </si>
+  <si>
+    <t>PYRO_PWR_V_SENSE</t>
+  </si>
+  <si>
+    <t>SERCOM I/O</t>
+  </si>
+  <si>
+    <t>ANALOG I/O</t>
+  </si>
+  <si>
+    <t>PYRO_PWR_I_SENSE</t>
+  </si>
+  <si>
+    <t>HYDRA_3V3_V_SENSE</t>
+  </si>
+  <si>
+    <t>HYDRA_3V3_I_SENSE</t>
+  </si>
+  <si>
+    <t>VCC_V_SENSE</t>
+  </si>
+  <si>
+    <t>INT_3V3_V_SENSE</t>
+  </si>
+  <si>
+    <t>OUTPUT_V_SENSE</t>
+  </si>
+  <si>
+    <t>VBAT_V_SENSE</t>
+  </si>
+  <si>
+    <t>LORA_nRST</t>
+  </si>
+  <si>
+    <t>BAT_I_SENSE</t>
   </si>
 </sst>
 </file>
@@ -417,14 +459,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,258 +818,270 @@
     <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="J2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4">
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="K5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" t="s">
         <v>8</v>
       </c>
       <c r="H7">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H8">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>3.6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" t="s">
         <v>8</v>
       </c>
       <c r="H11">
         <v>3.6</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H12">
         <v>3.6</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1039,18 +1093,18 @@
         <v>3.6</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -1062,78 +1116,84 @@
         <v>3.6</v>
       </c>
       <c r="J14" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>3.6</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16">
-        <v>3.6</v>
-      </c>
-      <c r="J16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H17">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -1144,13 +1204,16 @@
       <c r="H18">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -1161,16 +1224,19 @@
       <c r="H19">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -1178,68 +1244,62 @@
       <c r="H20">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
         <v>8</v>
       </c>
       <c r="H21">
         <v>3.6</v>
       </c>
-      <c r="J21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H22">
         <v>3.6</v>
       </c>
       <c r="J22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -1251,18 +1311,21 @@
         <v>3.6</v>
       </c>
       <c r="J23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -1274,18 +1337,18 @@
         <v>3.6</v>
       </c>
       <c r="J24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -1297,201 +1360,209 @@
         <v>3.6</v>
       </c>
       <c r="J25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>3.6</v>
+      </c>
+      <c r="J26" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>38</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="F26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="K27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>39</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>52</v>
       </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>40</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>53</v>
       </c>
-      <c r="F28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>41</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>54</v>
       </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>42</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>56</v>
       </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>43</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="K32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>44</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>58</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>48</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>32</v>
       </c>
-      <c r="G32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>45</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>50</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>60</v>
       </c>
-      <c r="G33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>46</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>61</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>62</v>
       </c>
-      <c r="G34" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>49</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35">
-        <v>5</v>
-      </c>
-      <c r="J35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>50</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -1501,276 +1572,301 @@
         <v>5</v>
       </c>
       <c r="J36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="J37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>51</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>20</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>68</v>
       </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>52</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>71</v>
       </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>53</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>74</v>
       </c>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="G40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>54</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>75</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40">
-        <v>5</v>
-      </c>
-      <c r="J40" t="s">
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+      <c r="J41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>55</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G41" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41">
-        <v>5</v>
-      </c>
-      <c r="J41" t="s">
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="J42" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>56</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42">
-        <v>5</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43">
+        <v>5</v>
+      </c>
+      <c r="J43" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>57</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>82</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>83</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>20</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>68</v>
       </c>
-      <c r="G43" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H43">
-        <v>5</v>
-      </c>
-      <c r="J43" s="6" t="s">
+      <c r="G44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="J44" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E45" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G44" t="s">
-        <v>8</v>
-      </c>
-      <c r="H44">
-        <v>5</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="G45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="J45" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>59</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>86</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E46" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G45" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45">
-        <v>5</v>
-      </c>
-      <c r="J45" t="s">
+      <c r="G46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="J46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>60</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>87</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>32</v>
       </c>
-      <c r="G46" t="s">
-        <v>8</v>
-      </c>
-      <c r="H46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="L47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>61</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>88</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E48" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G47" t="s">
-        <v>8</v>
-      </c>
-      <c r="H47">
-        <v>5</v>
-      </c>
-      <c r="J47" t="s">
+      <c r="G48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="J48" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>62</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>89</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G48" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48">
-        <v>5</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="J49" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C35:G35"/>
+  <mergeCells count="4">
     <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
uploading to work on desktop
</commit_message>
<xml_diff>
--- a/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_LINK/STM32G473RET6_PINOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_LINK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AD3A49-2D60-44C2-817A-37A83A6D2C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6ABD84-5251-4941-8C3A-8282945E9282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
+    <workbookView xWindow="588" yWindow="384" windowWidth="17280" windowHeight="10044" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="125">
   <si>
     <t>SPI</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>BAT_I_SENSE</t>
+  </si>
+  <si>
+    <t>TBC (RFD900)</t>
   </si>
 </sst>
 </file>
@@ -803,33 +806,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J1" s="6" t="s">
         <v>90</v>
       </c>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -864,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -881,7 +884,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -904,7 +907,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>9</v>
       </c>
@@ -927,7 +930,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -947,7 +950,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>11</v>
       </c>
@@ -967,7 +970,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>12</v>
       </c>
@@ -987,7 +990,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>13</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>14</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>17</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>18</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>19</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>21</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>22</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>23</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>24</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>25</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>26</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>30</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>33</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>34</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>35</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>36</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>37</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>38</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>39</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>40</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>41</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>42</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>43</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>44</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>45</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>46</v>
       </c>
@@ -1554,7 +1557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>49</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>50</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>51</v>
       </c>
@@ -1618,8 +1621,11 @@
       <c r="H38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>52</v>
       </c>
@@ -1638,8 +1644,11 @@
       <c r="H39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>53</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>54</v>
       </c>
@@ -1682,7 +1691,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>55</v>
       </c>
@@ -1702,7 +1711,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>56</v>
       </c>
@@ -1723,7 +1732,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>57</v>
       </c>
@@ -1749,7 +1758,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>58</v>
       </c>
@@ -1772,7 +1781,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>59</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>60</v>
       </c>
@@ -1815,7 +1824,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>61</v>
       </c>
@@ -1838,7 +1847,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>62</v>
       </c>

</xml_diff>